<commit_message>
Create new tables for account data
</commit_message>
<xml_diff>
--- a/src/resource/account/accountdb.xlsx
+++ b/src/resource/account/accountdb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="balancesheet" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="1255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="1256">
   <si>
     <t>流动资产</t>
   </si>
@@ -4094,55 +4094,56 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
+    <t>其他不涉及现金收支的投资和筹资活动金额</t>
+  </si>
+  <si>
+    <t>amount of other investment and financing activities that do not involve cash payments</t>
+  </si>
+  <si>
+    <t>beginperiodcash</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>减:现金的期初余额</t>
+  </si>
+  <si>
+    <t>endperiodcashequivalent</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>beginperiodcashequivalen</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>减：现金等价物的期初余额</t>
+  </si>
+  <si>
+    <t>cashequivalentnetincome</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>overallsalestab</t>
+  </si>
+  <si>
+    <t>overallcosttab</t>
+  </si>
+  <si>
+    <t>opsprofittab</t>
+  </si>
+  <si>
+    <t>利润</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>beginperiodcash</t>
+  </si>
+  <si>
+    <t>endperiodcash</t>
+  </si>
+  <si>
     <t>financeleasefixedasset</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他不涉及现金收支的投资和筹资活动金额</t>
-  </si>
-  <si>
-    <t>amount of other investment and financing activities that do not involve cash payments</t>
-  </si>
-  <si>
-    <t>endperiodcash</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>beginperiodcash</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>减:现金的期初余额</t>
-  </si>
-  <si>
-    <t>endperiodcashequivalent</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>beginperiodcashequivalen</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>减：现金等价物的期初余额</t>
-  </si>
-  <si>
-    <t>cashequivalentnetincome</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>overallsalestab</t>
-  </si>
-  <si>
-    <t>overallcosttab</t>
-  </si>
-  <si>
-    <t>opsprofittab</t>
-  </si>
-  <si>
-    <t>利润</t>
-  </si>
-  <si>
-    <t>profit</t>
   </si>
 </sst>
 </file>
@@ -4583,13 +4584,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E125" sqref="C125:E125"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
@@ -7461,14 +7463,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
   </cols>
@@ -7545,7 +7547,7 @@
         <v>379</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>565</v>
@@ -7916,7 +7918,7 @@
         <v>384</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>565</v>
@@ -8440,7 +8442,7 @@
         <v>315</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>565</v>
@@ -8635,13 +8637,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>565</v>
@@ -9132,14 +9134,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136:C136"/>
+    <sheetView topLeftCell="B196" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85:C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="94.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -10578,6 +10580,9 @@
       <c r="B86" t="s">
         <v>1069</v>
       </c>
+      <c r="C86" t="s">
+        <v>1067</v>
+      </c>
       <c r="D86" t="s">
         <v>564</v>
       </c>
@@ -10609,6 +10614,9 @@
       <c r="B88" t="s">
         <v>440</v>
       </c>
+      <c r="C88" t="s">
+        <v>1070</v>
+      </c>
       <c r="D88" t="s">
         <v>564</v>
       </c>
@@ -10708,6 +10716,9 @@
       <c r="B94" t="s">
         <v>333</v>
       </c>
+      <c r="C94" t="s">
+        <v>1075</v>
+      </c>
       <c r="D94" t="s">
         <v>564</v>
       </c>
@@ -11585,6 +11596,9 @@
       <c r="B146" t="s">
         <v>1152</v>
       </c>
+      <c r="C146" t="s">
+        <v>1150</v>
+      </c>
       <c r="D146" t="s">
         <v>564</v>
       </c>
@@ -12416,7 +12430,7 @@
         <v>463</v>
       </c>
       <c r="C195" t="s">
-        <v>1240</v>
+        <v>1255</v>
       </c>
       <c r="D195" t="s">
         <v>564</v>
@@ -12427,10 +12441,13 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="8" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B196" t="s">
         <v>1241</v>
       </c>
-      <c r="B196" t="s">
-        <v>1242</v>
+      <c r="C196" t="s">
+        <v>1255</v>
       </c>
       <c r="D196" t="s">
         <v>564</v>
@@ -12447,7 +12464,7 @@
         <v>464</v>
       </c>
       <c r="C197" t="s">
-        <v>1243</v>
+        <v>1254</v>
       </c>
       <c r="D197" t="s">
         <v>564</v>
@@ -12464,7 +12481,7 @@
         <v>465</v>
       </c>
       <c r="C198" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="D198" t="s">
         <v>564</v>
@@ -12475,13 +12492,13 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="8" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B199" t="s">
         <v>465</v>
       </c>
       <c r="C199" t="s">
-        <v>1244</v>
+        <v>1253</v>
       </c>
       <c r="D199" t="s">
         <v>564</v>
@@ -12498,7 +12515,7 @@
         <v>466</v>
       </c>
       <c r="C200" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D200" t="s">
         <v>564</v>
@@ -12515,7 +12532,7 @@
         <v>467</v>
       </c>
       <c r="C201" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="D201" t="s">
         <v>564</v>
@@ -12526,13 +12543,13 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="8" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B202" t="s">
         <v>467</v>
       </c>
       <c r="C202" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="D202" t="s">
         <v>564</v>
@@ -12549,7 +12566,7 @@
         <v>338</v>
       </c>
       <c r="C203" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="D203" t="s">
         <v>564</v>
@@ -12566,7 +12583,7 @@
         <v>338</v>
       </c>
       <c r="C204" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="D204" t="s">
         <v>564</v>

</xml_diff>